<commit_message>
add room filter to test file
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Personajes"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>Atracción</t>
   </si>
@@ -133,9 +133,15 @@
     <t>Resultado</t>
   </si>
   <si>
+    <t>Sala</t>
+  </si>
+  <si>
     <t>Una llave deseando ser introducida en una cerradura.</t>
   </si>
   <si>
+    <t>sala-de-prueba</t>
+  </si>
+  <si>
     <t>Una antorcha encendida.</t>
   </si>
   <si>
@@ -143,9 +149,6 @@
   </si>
   <si>
     <t>Jugador</t>
-  </si>
-  <si>
-    <t>Sala</t>
   </si>
   <si>
     <t>Equipado</t>
@@ -605,42 +608,42 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -663,10 +666,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -689,10 +692,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -723,14 +726,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -740,13 +744,19 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -759,16 +769,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -784,6 +795,9 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
@@ -796,7 +810,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -811,7 +828,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>